<commit_message>
Update on 29 April
</commit_message>
<xml_diff>
--- a/DB and Documents/WASHB_DRAFT_Mathernal.xlsx
+++ b/DB and Documents/WASHB_DRAFT_Mathernal.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8287" uniqueCount="2562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8287" uniqueCount="2581">
   <si>
     <t>SLNo</t>
   </si>
@@ -9872,6 +9872,63 @@
   </si>
   <si>
     <t>msgBhv</t>
+  </si>
+  <si>
+    <t>q_207_1</t>
+  </si>
+  <si>
+    <t>q_207_2</t>
+  </si>
+  <si>
+    <t>q_207_3</t>
+  </si>
+  <si>
+    <t>q_207_4</t>
+  </si>
+  <si>
+    <t>q_207_5</t>
+  </si>
+  <si>
+    <t>q_207_6</t>
+  </si>
+  <si>
+    <t>q_207_7</t>
+  </si>
+  <si>
+    <t>q_207_8</t>
+  </si>
+  <si>
+    <t>q_207_9</t>
+  </si>
+  <si>
+    <t>q_207_10</t>
+  </si>
+  <si>
+    <t>q_403_1</t>
+  </si>
+  <si>
+    <t>q_403_2</t>
+  </si>
+  <si>
+    <t>q_403_4</t>
+  </si>
+  <si>
+    <t>q_403_5</t>
+  </si>
+  <si>
+    <t>q_403_6</t>
+  </si>
+  <si>
+    <t>q_403_7</t>
+  </si>
+  <si>
+    <t>q_403_8</t>
+  </si>
+  <si>
+    <t>q_403_9</t>
+  </si>
+  <si>
+    <t>q_403_3</t>
   </si>
 </sst>
 </file>
@@ -11640,8 +11697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DK481"/>
   <sheetViews>
-    <sheetView topLeftCell="A393" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -13859,11 +13916,11 @@
       <c r="B54" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>759</v>
+      <c r="C54" s="84" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D54" s="84" t="s">
+        <v>760</v>
       </c>
       <c r="E54" s="59" t="s">
         <v>136</v>
@@ -13886,7 +13943,7 @@
       <c r="U54" s="83"/>
       <c r="V54" s="83" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('53', 'q_207','frmsinglechoice', 'tblMainQuesSc','207.MZ Pvi mßv‡n Avcbvi Amy¯’Zvi Rb¨, Avcwb wK †Kvb Wv³vi ev Ab¨ ‡Kvb wPwKrm‡Ki civgk© wb‡q‡Qb?hw` nu¨v nq: Kvi Kv‡Q Avcwb civgk© wb‡q‡Qb?†cÖve Kiæb: Ab¨ Kvi Kv‡Q Avcwb civgk© wb‡q‡Qb ?','207.In the past 4  weeks, did you consult a doctor or other professional or traditional health worker because you yourself were sick? IF YES: Whom did you consult?','','msg301','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('53', 'q_207','frmmultiplechoice', 'tblMainQuesMc','207.MZ Pvi mßv‡n Avcbvi Amy¯’Zvi Rb¨, Avcwb wK †Kvb Wv³vi ev Ab¨ ‡Kvb wPwKrm‡Ki civgk© wb‡q‡Qb?hw` nu¨v nq: Kvi Kv‡Q Avcwb civgk© wb‡q‡Qb?†cÖve Kiæb: Ab¨ Kvi Kv‡Q Avcwb civgk© wb‡q‡Qb ?','207.In the past 4  weeks, did you consult a doctor or other professional or traditional health worker because you yourself were sick? IF YES: Whom did you consult?','','msg301','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="55" spans="1:22" s="57" customFormat="1" ht="31.5">
@@ -14915,11 +14972,11 @@
       <c r="B81" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C81" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>759</v>
+      <c r="C81" s="84" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D81" s="84" t="s">
+        <v>760</v>
       </c>
       <c r="E81" s="59" t="s">
         <v>2400</v>
@@ -14942,7 +14999,7 @@
       <c r="U81" s="83"/>
       <c r="V81" s="83" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('80', 'q_403','frmsinglechoice', 'tblMainQuesSc','403.GB ev”Pv (ev”Pvi bvg) hLb M‡f©/†c‡U wQj, ZLb Mf©Kvjxb †gwW‡Kj †PKAv‡ci Rb¨ Avcwb Kv‡K †`wL‡qwQ‡jb? (DËi nu¨v n‡j) Kv‡K †`wL‡qwQ‡jb?','403.When you were pregnant with this child (NAME), did you see anyone for an antenatal check?IF YES: Whom did you see?Anyone else?','','q_404','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('80', 'q_403','frmmultiplechoice', 'tblMainQuesMc','403.GB ev”Pv (ev”Pvi bvg) hLb M‡f©/†c‡U wQj, ZLb Mf©Kvjxb †gwW‡Kj †PKAv‡ci Rb¨ Avcwb Kv‡K †`wL‡qwQ‡jb? (DËi nu¨v n‡j) Kv‡K †`wL‡qwQ‡jb?','403.When you were pregnant with this child (NAME), did you see anyone for an antenatal check?IF YES: Whom did you see?Anyone else?','','q_404','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="82" spans="1:22" s="57" customFormat="1" ht="31.5">
@@ -30120,7 +30177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1256" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G1274"/>
     </sheetView>
   </sheetViews>
@@ -33635,8 +33692,8 @@
       <c r="A162" s="83">
         <v>161</v>
       </c>
-      <c r="B162" s="6" t="s">
-        <v>117</v>
+      <c r="B162" s="84" t="s">
+        <v>2562</v>
       </c>
       <c r="C162" s="60" t="s">
         <v>474</v>
@@ -33649,15 +33706,15 @@
       </c>
       <c r="G162" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('161','q_207', 'A.NO ONE CONSULTED ','K.Kv‡iv civgk© †bq wb','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('161','q_207_1', 'A.NO ONE CONSULTED ','K.Kv‡iv civgk© †bq wb','1','');</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="25.5">
       <c r="A163" s="83">
         <v>162</v>
       </c>
-      <c r="B163" s="6" t="s">
-        <v>117</v>
+      <c r="B163" s="84" t="s">
+        <v>2563</v>
       </c>
       <c r="C163" s="60" t="s">
         <v>475</v>
@@ -33665,20 +33722,20 @@
       <c r="D163" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="E163">
-        <v>2</v>
+      <c r="E163" s="83">
+        <v>1</v>
       </c>
       <c r="G163" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('162','q_207', 'B.DOCTOR','L.Wv³vi','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('162','q_207_2', 'B.DOCTOR','L.Wv³vi','1','');</v>
       </c>
     </row>
     <row r="164" spans="1:7" ht="25.5">
       <c r="A164" s="83">
         <v>163</v>
       </c>
-      <c r="B164" s="6" t="s">
-        <v>117</v>
+      <c r="B164" s="84" t="s">
+        <v>2564</v>
       </c>
       <c r="C164" s="60" t="s">
         <v>476</v>
@@ -33686,20 +33743,20 @@
       <c r="D164" s="45" t="s">
         <v>486</v>
       </c>
-      <c r="E164">
-        <v>3</v>
+      <c r="E164" s="83">
+        <v>1</v>
       </c>
       <c r="G164" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('163','q_207', 'C.NURSE/ MIDWIFE ','M.bvm©/ avÎx','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('163','q_207_3', 'C.NURSE/ MIDWIFE ','M.bvm©/ avÎx','1','');</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="25.5">
       <c r="A165" s="83">
         <v>164</v>
       </c>
-      <c r="B165" s="6" t="s">
-        <v>117</v>
+      <c r="B165" s="84" t="s">
+        <v>2565</v>
       </c>
       <c r="C165" s="60" t="s">
         <v>477</v>
@@ -33707,20 +33764,20 @@
       <c r="D165" s="10" t="s">
         <v>487</v>
       </c>
-      <c r="E165">
-        <v>4</v>
+      <c r="E165" s="83">
+        <v>1</v>
       </c>
       <c r="G165" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('164','q_207', 'D.Govt. Health Worker','N.miKvix  ¯^v¯’¨Kgx©','4','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('164','q_207_4', 'D.Govt. Health Worker','N.miKvix  ¯^v¯’¨Kgx©','1','');</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="25.5">
       <c r="A166" s="83">
         <v>165</v>
       </c>
-      <c r="B166" s="6" t="s">
-        <v>117</v>
+      <c r="B166" s="84" t="s">
+        <v>2566</v>
       </c>
       <c r="C166" s="60" t="s">
         <v>478</v>
@@ -33728,20 +33785,20 @@
       <c r="D166" s="10" t="s">
         <v>488</v>
       </c>
-      <c r="E166">
-        <v>5</v>
+      <c r="E166" s="83">
+        <v>1</v>
       </c>
       <c r="G166" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('165','q_207', 'E.NGO Health Worker','O.Gb.wR.I ¯^v¯’¨Kgx©','5','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('165','q_207_5', 'E.NGO Health Worker','O.Gb.wR.I ¯^v¯’¨Kgx©','1','');</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="25.5">
       <c r="A167" s="83">
         <v>166</v>
       </c>
-      <c r="B167" s="6" t="s">
-        <v>117</v>
+      <c r="B167" s="84" t="s">
+        <v>2567</v>
       </c>
       <c r="C167" s="60" t="s">
         <v>479</v>
@@ -33749,20 +33806,20 @@
       <c r="D167" s="10" t="s">
         <v>489</v>
       </c>
-      <c r="E167">
-        <v>6</v>
+      <c r="E167" s="83">
+        <v>1</v>
       </c>
       <c r="G167" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('166','q_207', 'F.COUNSELLOR','P.civgk© `vZv','6','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('166','q_207_6', 'F.COUNSELLOR','P.civgk© `vZv','1','');</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="25.5">
       <c r="A168" s="83">
         <v>167</v>
       </c>
-      <c r="B168" s="6" t="s">
-        <v>117</v>
+      <c r="B168" s="84" t="s">
+        <v>2568</v>
       </c>
       <c r="C168" s="60" t="s">
         <v>480</v>
@@ -33770,20 +33827,20 @@
       <c r="D168" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="E168">
-        <v>7</v>
+      <c r="E168" s="83">
+        <v>1</v>
       </c>
       <c r="G168" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('167','q_207', 'G.PHARMACIST','Q.Jla we‡µZv','7','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('167','q_207_7', 'G.PHARMACIST','Q.Jla we‡µZv','1','');</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="25.5">
       <c r="A169" s="83">
         <v>168</v>
       </c>
-      <c r="B169" s="6" t="s">
-        <v>117</v>
+      <c r="B169" s="84" t="s">
+        <v>2569</v>
       </c>
       <c r="C169" s="60" t="s">
         <v>481</v>
@@ -33791,20 +33848,20 @@
       <c r="D169" s="10" t="s">
         <v>491</v>
       </c>
-      <c r="E169">
-        <v>8</v>
+      <c r="E169" s="83">
+        <v>1</v>
       </c>
       <c r="G169" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('168','q_207', 'H.TRADITIONAL HEALER','R.mbvZb wPwKrmK','8','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('168','q_207_8', 'H.TRADITIONAL HEALER','R.mbvZb wPwKrmK','1','');</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="25.5">
       <c r="A170" s="83">
         <v>169</v>
       </c>
-      <c r="B170" s="6" t="s">
-        <v>117</v>
+      <c r="B170" s="84" t="s">
+        <v>2570</v>
       </c>
       <c r="C170" s="60" t="s">
         <v>482</v>
@@ -33812,20 +33869,20 @@
       <c r="D170" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="E170">
-        <v>9</v>
+      <c r="E170" s="83">
+        <v>1</v>
       </c>
       <c r="G170" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('169','q_207', 'I.TRADITIONAL BIRTH ATTENDANT','S.`vB','9','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('169','q_207_9', 'I.TRADITIONAL BIRTH ATTENDANT','S.`vB','1','');</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="25.5">
       <c r="A171" s="83">
         <v>170</v>
       </c>
-      <c r="B171" s="6" t="s">
-        <v>117</v>
+      <c r="B171" s="84" t="s">
+        <v>2571</v>
       </c>
       <c r="C171" s="60" t="s">
         <v>483</v>
@@ -33833,15 +33890,15 @@
       <c r="D171" s="10" t="s">
         <v>493</v>
       </c>
-      <c r="E171">
-        <v>10</v>
+      <c r="E171" s="83">
+        <v>1</v>
       </c>
       <c r="F171" s="58" t="s">
         <v>2478</v>
       </c>
       <c r="G171" s="18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('170','q_207', 'X.OTHER','T.Ab¨vb¨','10','q_207_other');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('170','q_207_10', 'X.OTHER','T.Ab¨vb¨','1','q_207_other');</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="25.5">
@@ -34496,8 +34553,8 @@
       <c r="A202" s="83">
         <v>201</v>
       </c>
-      <c r="B202" s="6" t="s">
-        <v>189</v>
+      <c r="B202" s="84" t="s">
+        <v>2572</v>
       </c>
       <c r="C202" s="60" t="s">
         <v>543</v>
@@ -34510,15 +34567,15 @@
       </c>
       <c r="G202" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('201','q_403', '1.NO ONE','1.KvD‡K bv','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('201','q_403_1', '1.NO ONE','1.KvD‡K bv','1','');</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="25.5">
       <c r="A203" s="83">
         <v>202</v>
       </c>
-      <c r="B203" s="6" t="s">
-        <v>189</v>
+      <c r="B203" s="84" t="s">
+        <v>2573</v>
       </c>
       <c r="C203" s="60" t="s">
         <v>545</v>
@@ -34526,20 +34583,20 @@
       <c r="D203" s="10" t="s">
         <v>546</v>
       </c>
-      <c r="E203" s="54">
-        <v>2</v>
+      <c r="E203" s="89">
+        <v>1</v>
       </c>
       <c r="G203" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('202','q_403', '2.DOCTOR','2.Wv³vi','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('202','q_403_2', '2.DOCTOR','2.Wv³vi','1','');</v>
       </c>
     </row>
     <row r="204" spans="1:7" ht="25.5">
       <c r="A204" s="83">
         <v>203</v>
       </c>
-      <c r="B204" s="6" t="s">
-        <v>189</v>
+      <c r="B204" s="84" t="s">
+        <v>2580</v>
       </c>
       <c r="C204" s="60" t="s">
         <v>547</v>
@@ -34547,20 +34604,20 @@
       <c r="D204" s="10" t="s">
         <v>548</v>
       </c>
-      <c r="E204" s="54">
-        <v>3</v>
+      <c r="E204" s="89">
+        <v>1</v>
       </c>
       <c r="G204" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('203','q_403', '3.OBSTETRICIAN/GYNAECOLOGIST','3.avÎxwe`¨vwekvi`/¯¿x†ivMwekvi`','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('203','q_403_3', '3.OBSTETRICIAN/GYNAECOLOGIST','3.avÎxwe`¨vwekvi`/¯¿x†ivMwekvi`','1','');</v>
       </c>
     </row>
     <row r="205" spans="1:7" ht="25.5">
       <c r="A205" s="83">
         <v>204</v>
       </c>
-      <c r="B205" s="6" t="s">
-        <v>189</v>
+      <c r="B205" s="84" t="s">
+        <v>2574</v>
       </c>
       <c r="C205" s="60" t="s">
         <v>549</v>
@@ -34568,20 +34625,20 @@
       <c r="D205" s="10" t="s">
         <v>550</v>
       </c>
-      <c r="E205" s="54">
-        <v>4</v>
+      <c r="E205" s="89">
+        <v>1</v>
       </c>
       <c r="G205" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('204','q_403', '4.NURSE/MIDWIFE','4.†mweKv/avÎx','4','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('204','q_403_4', '4.NURSE/MIDWIFE','4.†mweKv/avÎx','1','');</v>
       </c>
     </row>
     <row r="206" spans="1:7" ht="25.5">
       <c r="A206" s="83">
         <v>205</v>
       </c>
-      <c r="B206" s="6" t="s">
-        <v>189</v>
+      <c r="B206" s="84" t="s">
+        <v>2575</v>
       </c>
       <c r="C206" s="60" t="s">
         <v>551</v>
@@ -34589,20 +34646,20 @@
       <c r="D206" s="16" t="s">
         <v>552</v>
       </c>
-      <c r="E206" s="54">
-        <v>5</v>
+      <c r="E206" s="89">
+        <v>1</v>
       </c>
       <c r="G206" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('205','q_403', '5.FWV/CSBA/SBA/MA/SACMO','5.miKvix ¯^v¯’¨ Kg©x','5','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('205','q_403_5', '5.FWV/CSBA/SBA/MA/SACMO','5.miKvix ¯^v¯’¨ Kg©x','1','');</v>
       </c>
     </row>
     <row r="207" spans="1:7" ht="25.5">
       <c r="A207" s="83">
         <v>206</v>
       </c>
-      <c r="B207" s="6" t="s">
-        <v>189</v>
+      <c r="B207" s="84" t="s">
+        <v>2576</v>
       </c>
       <c r="C207" s="60" t="s">
         <v>553</v>
@@ -34610,20 +34667,20 @@
       <c r="D207" s="10" t="s">
         <v>554</v>
       </c>
-      <c r="E207" s="54">
-        <v>6</v>
+      <c r="E207" s="89">
+        <v>1</v>
       </c>
       <c r="G207" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('206','q_403', '6.NGO HEALTH WORKER ','6.Gb.wR.I.¯^v¯’¨ Kg©x','6','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('206','q_403_6', '6.NGO HEALTH WORKER ','6.Gb.wR.I.¯^v¯’¨ Kg©x','1','');</v>
       </c>
     </row>
     <row r="208" spans="1:7" ht="25.5">
       <c r="A208" s="83">
         <v>207</v>
       </c>
-      <c r="B208" s="6" t="s">
-        <v>189</v>
+      <c r="B208" s="84" t="s">
+        <v>2577</v>
       </c>
       <c r="C208" s="60" t="s">
         <v>555</v>
@@ -34631,20 +34688,20 @@
       <c r="D208" s="10" t="s">
         <v>556</v>
       </c>
-      <c r="E208" s="54">
-        <v>7</v>
+      <c r="E208" s="89">
+        <v>1</v>
       </c>
       <c r="G208" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('207','q_403', '7.VILLAGE DOCTOR','7.cjøx wPwKrmK','7','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('207','q_403_7', '7.VILLAGE DOCTOR','7.cjøx wPwKrmK','1','');</v>
       </c>
     </row>
     <row r="209" spans="1:7" ht="25.5">
       <c r="A209" s="83">
         <v>208</v>
       </c>
-      <c r="B209" s="6" t="s">
-        <v>189</v>
+      <c r="B209" s="84" t="s">
+        <v>2578</v>
       </c>
       <c r="C209" s="60" t="s">
         <v>557</v>
@@ -34652,20 +34709,20 @@
       <c r="D209" s="10" t="s">
         <v>558</v>
       </c>
-      <c r="E209" s="54">
-        <v>8</v>
+      <c r="E209" s="89">
+        <v>1</v>
       </c>
       <c r="G209" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('208','q_403', '8.TRADITIONAL BIRTH ATTENDANT','8.`vB','8','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('208','q_403_8', '8.TRADITIONAL BIRTH ATTENDANT','8.`vB','1','');</v>
       </c>
     </row>
     <row r="210" spans="1:7" ht="25.5">
       <c r="A210" s="83">
         <v>209</v>
       </c>
-      <c r="B210" s="6" t="s">
-        <v>189</v>
+      <c r="B210" s="84" t="s">
+        <v>2579</v>
       </c>
       <c r="C210" s="60" t="s">
         <v>559</v>
@@ -34673,15 +34730,15 @@
       <c r="D210" s="10" t="s">
         <v>560</v>
       </c>
-      <c r="E210" s="54">
-        <v>9</v>
+      <c r="E210" s="89">
+        <v>1</v>
       </c>
       <c r="F210" s="58" t="s">
         <v>2484</v>
       </c>
       <c r="G210" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('209','q_403', '9.OTHER','9.Ab¨vb¨','9','q_403_other');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('209','q_403_9', '9.OTHER','9.Ab¨vb¨','1','q_403_other');</v>
       </c>
     </row>
     <row r="211" spans="1:7" ht="25.5">

</xml_diff>